<commit_message>
feat: upgrade to dcat version 2
</commit_message>
<xml_diff>
--- a/molgenis-api-fair/src/test/resources/FDP_test_data.xlsx
+++ b/molgenis-api-fair/src/test/resources/FDP_test_data.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-api-fair/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53C9133-DD86-6549-AB2B-8C80CCD3A71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40060" yWindow="-5600" windowWidth="25600" windowHeight="15540" tabRatio="621" activeTab="3"/>
+    <workbookView xWindow="32960" yWindow="-7680" windowWidth="21360" windowHeight="16560" tabRatio="621" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fdp_Metadata" sheetId="8" r:id="rId1"/>
     <sheet name="fdp_Catalog" sheetId="9" r:id="rId2"/>
     <sheet name="fdp_Dataset" sheetId="10" r:id="rId3"/>
     <sheet name="fdp_IRI" sheetId="13" r:id="rId4"/>
+    <sheet name="fdp_Publisher" sheetId="14" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>description</t>
   </si>
@@ -45,9 +52,6 @@
     <t>rights</t>
   </si>
   <si>
-    <t>metadataIdentifier</t>
-  </si>
-  <si>
     <t>issued</t>
   </si>
   <si>
@@ -129,14 +133,23 @@
     <t>http://example.org</t>
   </si>
   <si>
-    <t>http://molgenis01.gcc.rug.nl/fdp/catalogue</t>
+    <t>molgenis</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>MOLGENIS</t>
+  </si>
+  <si>
+    <t>2020-09-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -196,7 +209,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,6 +220,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -219,6 +233,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -543,41 +565,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="62.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="3" customWidth="1"/>
-    <col min="9" max="9" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="21" width="10.5" customWidth="1"/>
-    <col min="22" max="24" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="20" width="10.5" customWidth="1"/>
+    <col min="21" max="23" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1">
+    <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -589,60 +609,51 @@
         <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1">
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -654,39 +665,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="38.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="27" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1">
+    <row r="1" spans="1:13" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -698,16 +708,16 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>12</v>
@@ -715,54 +725,48 @@
       <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2">
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -775,40 +779,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="27" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10.5" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1">
+    <row r="1" spans="1:15" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -820,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>16</v>
@@ -843,51 +846,45 @@
       <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -900,21 +897,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -922,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -930,13 +927,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -945,4 +942,38 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B883EC-A7D4-264A-A2FC-25E3966E9A46}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(api-fdp): add RightsStatement to the model
</commit_message>
<xml_diff>
--- a/molgenis-api-fair/src/test/resources/FDP_test_data.xlsx
+++ b/molgenis-api-fair/src/test/resources/FDP_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-api-fair/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53C9133-DD86-6549-AB2B-8C80CCD3A71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E519D680-147D-0943-B432-BCD086A8F806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32960" yWindow="-7680" windowWidth="21360" windowHeight="16560" tabRatio="621" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31340" yWindow="-8940" windowWidth="26800" windowHeight="16560" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fdp_Metadata" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>description</t>
   </si>
@@ -143,13 +143,16 @@
   </si>
   <si>
     <t>2020-09-23</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -158,6 +161,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -169,18 +173,27 @@
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +222,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,6 +234,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -568,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -649,6 +663,9 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
+      <c r="J2" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="K2" t="s">
         <v>25</v>
       </c>
@@ -669,7 +686,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -753,6 +770,9 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>27</v>
@@ -782,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -871,6 +891,9 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="L2">
         <v>1</v>

</xml_diff>